<commit_message>
updating registry tools comparison
</commit_message>
<xml_diff>
--- a/linkeddataregistries/Comparatif_outils_registre.xlsx
+++ b/linkeddataregistries/Comparatif_outils_registre.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feliachi\INSIDE\linkeddataregistries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\grellets\Travail\GitHub\INSIDE-information-systems\EnvironmentalSemanticWeb\linkeddataregistries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6870" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6876" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EN" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
   <si>
     <t>proper linked data approach</t>
   </si>
@@ -468,12 +468,6 @@
     <t>possible,  throught context declaration</t>
   </si>
   <si>
-    <t>possible,   les ontolgies utilisées localement peuvent être alignées avec des ontologies externes</t>
-  </si>
-  <si>
-    <t>possible,  les ontolgies utilisées localement peuvent être alignées</t>
-  </si>
-  <si>
     <t xml:space="preserve">possible, par le formulaire d'edition ou par le chargement d'un fichier de MAJ </t>
   </si>
   <si>
@@ -495,21 +489,12 @@
     <t>vérification de l' @id seulement</t>
   </si>
   <si>
-    <t>pas fournie</t>
-  </si>
-  <si>
-    <t>V7 pour ce realese</t>
-  </si>
-  <si>
     <t xml:space="preserve">oui, selon les derniers tests </t>
   </si>
   <si>
     <t>continu</t>
   </si>
   <si>
-    <t>Par Github:  "issues" et de mande de "merge"+ contacte direct avec l'équipe de Dev</t>
-  </si>
-  <si>
     <t>depend de la configuration du serveur, le fait que les données sont transformées en RDF avant d'être stoqué en triple store doit être pris en compte</t>
   </si>
   <si>
@@ -558,9 +543,6 @@
     <t>quelques (2-3) état membres testant déploiement pour INSPIRE</t>
   </si>
   <si>
-    <t>ex: CSIRO, WMO, OGC NA, UK metoffice, uk defra/food ..</t>
-  </si>
-  <si>
     <t>nouvelle version dispo prochainement</t>
   </si>
   <si>
@@ -577,6 +559,36 @@
   </si>
   <si>
     <t>Github source + wiki maintenu par Epimorphics (anciens groupes W3C linked data, apache JENA, …)</t>
+  </si>
+  <si>
+    <t>Par Github:  "issues" et demande de "merge"+ contacte direct avec l'équipe de Dev</t>
+  </si>
+  <si>
+    <t>non, en cours de mise en place BRGM/Epimorphics</t>
+  </si>
+  <si>
+    <t>ukgovld 2.0</t>
+  </si>
+  <si>
+    <t>V8+ pour ce release</t>
+  </si>
+  <si>
+    <t>oui pour le contenu, internationalisation en cours pour la GUI</t>
+  </si>
+  <si>
+    <t>utilisés dans de nombreuses infrastructures en production (cf liste communautés plus haut)</t>
+  </si>
+  <si>
+    <t>possible,  les ontolgies/vocabulaires utilisés localement peuvent être alignés</t>
+  </si>
+  <si>
+    <t>possible,   les ontolgies/vocabulaires utilisées localement peuvent être alignés avec des ontologies/vocabulaires externes</t>
+  </si>
+  <si>
+    <t>en cours de developpement pour BRGM</t>
+  </si>
+  <si>
+    <t>ex: CSIRO, WMO, OGC NA, UK metoffice, uk defra/food, NOAA…</t>
   </si>
 </sst>
 </file>
@@ -719,7 +731,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -897,12 +909,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1091,7 +1097,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1111,20 +1117,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1466,22 +1478,22 @@
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="66.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="66.5546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="36" style="6" customWidth="1"/>
     <col min="5" max="5" width="43" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="4" t="s">
         <v>53</v>
       </c>
@@ -1489,14 +1501,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="6" t="s">
         <v>112</v>
       </c>
@@ -1504,8 +1516,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1519,9 +1531,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1531,9 +1543,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1541,9 +1553,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1553,9 +1565,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="12"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1563,9 +1575,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1575,9 +1587,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1585,57 +1597,57 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="11" t="s">
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="6" t="s">
         <v>117</v>
       </c>
@@ -1643,12 +1655,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="6" t="s">
         <v>113</v>
       </c>
@@ -1656,9 +1668,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1671,16 +1683,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="11"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
         <v>80</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1693,9 +1705,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1706,9 +1718,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="5" t="s">
         <v>145</v>
       </c>
@@ -1719,9 +1731,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1732,8 +1744,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1746,12 +1758,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="11" t="s">
+    <row r="24" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="6" t="s">
         <v>115</v>
       </c>
@@ -1759,12 +1771,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9" t="s">
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="4" t="s">
         <v>113</v>
       </c>
@@ -1772,11 +1784,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1789,9 +1801,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="11"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="5" t="s">
         <v>31</v>
       </c>
@@ -1802,9 +1814,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="11"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="5" t="s">
         <v>32</v>
       </c>
@@ -1812,9 +1824,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="11"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="5" t="s">
         <v>33</v>
       </c>
@@ -1825,9 +1837,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="11"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="5" t="s">
         <v>34</v>
       </c>
@@ -1838,56 +1850,56 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10" t="s">
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10" t="s">
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="12"/>
       <c r="E34" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="11" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1897,9 +1909,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="11"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="5" t="s">
         <v>95</v>
       </c>
@@ -1907,9 +1919,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="11"/>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="5" t="s">
         <v>40</v>
       </c>
@@ -1917,19 +1929,19 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="11" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
       <c r="E38" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="11" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="11"/>
+      <c r="B39" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1939,9 +1951,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="11"/>
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="5" t="s">
         <v>44</v>
       </c>
@@ -1949,19 +1961,19 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="11" t="s">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="12"/>
       <c r="E41" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8" t="s">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -1971,9 +1983,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1982,14 +1994,14 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="9"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="4" t="s">
         <v>113</v>
       </c>
@@ -1999,11 +2011,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B41:C41"/>
@@ -2019,18 +2038,11 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B42:B43"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2039,42 +2051,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="44" style="6" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="E1" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="6" t="s">
         <v>139</v>
       </c>
@@ -2082,8 +2094,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
       <c r="B3" s="6" t="s">
         <v>56</v>
       </c>
@@ -2094,27 +2106,27 @@
         <v>142</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+      <c r="B4" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12"/>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="6" t="s">
         <v>60</v>
       </c>
@@ -2122,27 +2134,27 @@
         <v>139</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="6" t="s">
         <v>63</v>
       </c>
@@ -2150,81 +2162,81 @@
         <v>139</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -2237,78 +2249,78 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+    <row r="14" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="6" t="s">
         <v>139</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13" t="s">
+      <c r="E18" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -2317,13 +2329,13 @@
       <c r="D19" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+      <c r="E19" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="6" t="s">
         <v>82</v>
       </c>
@@ -2331,12 +2343,12 @@
         <v>139</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="5" t="s">
         <v>105</v>
       </c>
@@ -2344,12 +2356,12 @@
         <v>139</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="4" t="s">
         <v>83</v>
       </c>
@@ -2360,8 +2372,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
         <v>85</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -2371,43 +2383,43 @@
         <v>87</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="6" t="s">
         <v>115</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13"/>
+      <c r="B25" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -2417,254 +2429,273 @@
         <v>139</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="12"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="12"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="12"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10" t="s">
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="13"/>
+      <c r="B33" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="C33" s="17"/>
+      <c r="D33" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="E34" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="12" t="s">
+      <c r="C34" s="14"/>
+      <c r="E34" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
+      <c r="B35" s="14" t="s">
         <v>91</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>92</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="12"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D36" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="12"/>
+    </row>
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="15"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="15"/>
+      <c r="B38" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="15"/>
+      <c r="B39" s="14" t="s">
         <v>96</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="12"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="6" t="s">
         <v>98</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15" t="s">
         <v>46</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>100</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="13"/>
+      <c r="D44" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="E44" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B22"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B31:C31"/>
@@ -2681,22 +2712,6 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>